<commit_message>
Uebersicht erweitert: Doc, Testing
</commit_message>
<xml_diff>
--- a/Dokumente/Lerngruppe_Uebersicht_v1.xlsx
+++ b/Dokumente/Lerngruppe_Uebersicht_v1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="96" windowWidth="20112" windowHeight="8256"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
     <sheet name="Teilnehmerliste" sheetId="2" r:id="rId2"/>
     <sheet name="Anwesenheit" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="49">
   <si>
     <t>KW</t>
   </si>
@@ -160,13 +160,16 @@
   </si>
   <si>
     <t>Stunden-Übersicht</t>
+  </si>
+  <si>
+    <t>PHPDoc, PHPUnit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,7 +363,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -434,7 +437,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -469,7 +471,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -645,25 +646,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -689,7 +690,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="4">
         <v>49</v>
       </c>
@@ -713,7 +714,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>50</v>
       </c>
@@ -737,7 +738,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>51</v>
       </c>
@@ -759,7 +760,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>52</v>
       </c>
@@ -781,7 +782,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -803,7 +804,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -825,7 +826,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -847,7 +848,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="10">
         <v>4</v>
       </c>
@@ -869,17 +870,19 @@
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="F10" s="17"/>
       <c r="G10" s="18"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -889,7 +892,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -905,19 +908,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1">
       <c r="A1" s="21" t="s">
         <v>16</v>
       </c>
@@ -928,7 +931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -939,7 +942,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -950,7 +953,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -961,7 +964,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -972,7 +975,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -983,7 +986,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -994,7 +997,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1071,7 +1074,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1198,21 +1201,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1">
       <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1">
       <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1254,7 +1257,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1263,7 +1266,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1272,7 +1275,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1281,7 +1284,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1290,7 +1293,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1299,7 +1302,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1308,7 +1311,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1317,7 +1320,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="19">
         <v>9</v>
       </c>
@@ -1326,7 +1329,7 @@
       </c>
       <c r="C12" s="19"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1335,7 +1338,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1344,7 +1347,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1353,7 +1356,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1362,7 +1365,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
@@ -1371,7 +1374,7 @@
       </c>
       <c r="C17" s="19"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1380,7 +1383,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -1389,7 +1392,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -1398,7 +1401,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -1407,7 +1410,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -1416,7 +1419,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -1425,7 +1428,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -1434,7 +1437,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -1443,7 +1446,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -1452,7 +1455,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="11">
         <v>24</v>
       </c>
@@ -1461,12 +1464,12 @@
       </c>
       <c r="C27" s="11"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" thickBot="1">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15" thickBot="1">
       <c r="A29" s="20" t="s">
         <v>2</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" thickBot="1">
       <c r="A30" s="5">
         <v>2</v>
       </c>
@@ -1488,7 +1491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" thickBot="1">
       <c r="A31" s="20" t="s">
         <v>16</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="5">
         <v>1</v>
       </c>
@@ -1508,7 +1511,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="2">
         <v>2</v>
       </c>
@@ -1517,7 +1520,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="2">
         <v>3</v>
       </c>
@@ -1526,7 +1529,7 @@
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="2">
         <v>4</v>
       </c>
@@ -1535,7 +1538,7 @@
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="2">
         <v>5</v>
       </c>
@@ -1544,7 +1547,7 @@
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="2">
         <v>6</v>
       </c>
@@ -1553,7 +1556,7 @@
       </c>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="2">
         <v>7</v>
       </c>
@@ -1562,7 +1565,7 @@
       </c>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="2">
         <v>8</v>
       </c>
@@ -1571,7 +1574,7 @@
       </c>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="19">
         <v>9</v>
       </c>
@@ -1580,7 +1583,7 @@
       </c>
       <c r="C40" s="19"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="2">
         <v>10</v>
       </c>
@@ -1589,7 +1592,7 @@
       </c>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="2">
         <v>11</v>
       </c>
@@ -1598,7 +1601,7 @@
       </c>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="2">
         <v>12</v>
       </c>
@@ -1607,7 +1610,7 @@
       </c>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="2">
         <v>13</v>
       </c>
@@ -1616,7 +1619,7 @@
       </c>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="19">
         <v>14</v>
       </c>
@@ -1625,7 +1628,7 @@
       </c>
       <c r="C45" s="19"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="2">
         <v>15</v>
       </c>
@@ -1634,7 +1637,7 @@
       </c>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="2">
         <v>16</v>
       </c>
@@ -1643,7 +1646,7 @@
       </c>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="2">
         <v>17</v>
       </c>
@@ -1652,7 +1655,7 @@
       </c>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="2">
         <v>18</v>
       </c>
@@ -1661,7 +1664,7 @@
       </c>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="2">
         <v>19</v>
       </c>
@@ -1670,7 +1673,7 @@
       </c>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="2">
         <v>20</v>
       </c>
@@ -1679,7 +1682,7 @@
       </c>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="2">
         <v>21</v>
       </c>
@@ -1688,7 +1691,7 @@
       </c>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="2">
         <v>22</v>
       </c>
@@ -1697,7 +1700,7 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="2">
         <v>23</v>
       </c>
@@ -1706,7 +1709,7 @@
       </c>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="2">
         <v>24</v>
       </c>
@@ -1715,8 +1718,8 @@
       </c>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="15" thickBot="1"/>
+    <row r="57" spans="1:3" ht="15" thickBot="1">
       <c r="A57" s="20" t="s">
         <v>2</v>
       </c>
@@ -1727,7 +1730,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="15" thickBot="1">
       <c r="A58" s="5">
         <v>3</v>
       </c>
@@ -1738,7 +1741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="15" thickBot="1">
       <c r="A59" s="20" t="s">
         <v>16</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="5">
         <v>1</v>
       </c>
@@ -1758,7 +1761,7 @@
       </c>
       <c r="C60" s="5"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="2">
         <v>2</v>
       </c>
@@ -1767,7 +1770,7 @@
       </c>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="2">
         <v>3</v>
       </c>
@@ -1776,7 +1779,7 @@
       </c>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="2">
         <v>4</v>
       </c>
@@ -1785,7 +1788,7 @@
       </c>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="2">
         <v>5</v>
       </c>
@@ -1794,7 +1797,7 @@
       </c>
       <c r="C64" s="2"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="2">
         <v>6</v>
       </c>
@@ -1803,7 +1806,7 @@
       </c>
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="2">
         <v>7</v>
       </c>
@@ -1812,7 +1815,7 @@
       </c>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="2">
         <v>8</v>
       </c>
@@ -1821,7 +1824,7 @@
       </c>
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="19">
         <v>9</v>
       </c>
@@ -1830,7 +1833,7 @@
       </c>
       <c r="C68" s="19"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="2">
         <v>10</v>
       </c>
@@ -1839,7 +1842,7 @@
       </c>
       <c r="C69" s="2"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="2">
         <v>11</v>
       </c>
@@ -1848,7 +1851,7 @@
       </c>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="2">
         <v>12</v>
       </c>
@@ -1857,7 +1860,7 @@
       </c>
       <c r="C71" s="2"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="2">
         <v>13</v>
       </c>
@@ -1866,7 +1869,7 @@
       </c>
       <c r="C72" s="2"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="19">
         <v>14</v>
       </c>
@@ -1875,7 +1878,7 @@
       </c>
       <c r="C73" s="19"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="2">
         <v>15</v>
       </c>
@@ -1884,7 +1887,7 @@
       </c>
       <c r="C74" s="2"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="2">
         <v>16</v>
       </c>
@@ -1893,7 +1896,7 @@
       </c>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="2">
         <v>17</v>
       </c>
@@ -1902,7 +1905,7 @@
       </c>
       <c r="C76" s="2"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="2">
         <v>18</v>
       </c>
@@ -1911,7 +1914,7 @@
       </c>
       <c r="C77" s="2"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="2">
         <v>19</v>
       </c>
@@ -1920,7 +1923,7 @@
       </c>
       <c r="C78" s="2"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="2">
         <v>20</v>
       </c>
@@ -1929,7 +1932,7 @@
       </c>
       <c r="C79" s="2"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="2">
         <v>21</v>
       </c>
@@ -1938,7 +1941,7 @@
       </c>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="2">
         <v>22</v>
       </c>
@@ -1947,7 +1950,7 @@
       </c>
       <c r="C81" s="2"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="2">
         <v>23</v>
       </c>
@@ -1956,7 +1959,7 @@
       </c>
       <c r="C82" s="2"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="2">
         <v>24</v>
       </c>
@@ -1965,8 +1968,8 @@
       </c>
       <c r="C83" s="2"/>
     </row>
-    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="15" thickBot="1"/>
+    <row r="85" spans="1:3" ht="15" thickBot="1">
       <c r="A85" s="20" t="s">
         <v>2</v>
       </c>
@@ -1977,7 +1980,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="15" thickBot="1">
       <c r="A86" s="5">
         <v>4</v>
       </c>
@@ -1988,7 +1991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="15" thickBot="1">
       <c r="A87" s="20" t="s">
         <v>16</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="5">
         <v>1</v>
       </c>
@@ -2008,7 +2011,7 @@
       </c>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="2">
         <v>2</v>
       </c>
@@ -2017,7 +2020,7 @@
       </c>
       <c r="C89" s="2"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" s="2">
         <v>3</v>
       </c>
@@ -2026,7 +2029,7 @@
       </c>
       <c r="C90" s="2"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="2">
         <v>4</v>
       </c>
@@ -2035,7 +2038,7 @@
       </c>
       <c r="C91" s="2"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="2">
         <v>5</v>
       </c>
@@ -2044,7 +2047,7 @@
       </c>
       <c r="C92" s="2"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" s="2">
         <v>6</v>
       </c>
@@ -2053,7 +2056,7 @@
       </c>
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" s="2">
         <v>7</v>
       </c>
@@ -2062,7 +2065,7 @@
       </c>
       <c r="C94" s="2"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" s="2">
         <v>8</v>
       </c>
@@ -2071,7 +2074,7 @@
       </c>
       <c r="C95" s="2"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="19">
         <v>9</v>
       </c>
@@ -2080,7 +2083,7 @@
       </c>
       <c r="C96" s="19"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" s="2">
         <v>10</v>
       </c>
@@ -2089,7 +2092,7 @@
       </c>
       <c r="C97" s="2"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" s="2">
         <v>11</v>
       </c>
@@ -2098,7 +2101,7 @@
       </c>
       <c r="C98" s="2"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" s="2">
         <v>12</v>
       </c>
@@ -2107,7 +2110,7 @@
       </c>
       <c r="C99" s="2"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" s="2">
         <v>13</v>
       </c>
@@ -2116,7 +2119,7 @@
       </c>
       <c r="C100" s="2"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" s="19">
         <v>14</v>
       </c>
@@ -2125,7 +2128,7 @@
       </c>
       <c r="C101" s="19"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" s="2">
         <v>15</v>
       </c>
@@ -2134,7 +2137,7 @@
       </c>
       <c r="C102" s="2"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" s="2">
         <v>16</v>
       </c>
@@ -2143,7 +2146,7 @@
       </c>
       <c r="C103" s="2"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" s="2">
         <v>17</v>
       </c>
@@ -2152,7 +2155,7 @@
       </c>
       <c r="C104" s="2"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" s="2">
         <v>18</v>
       </c>
@@ -2161,7 +2164,7 @@
       </c>
       <c r="C105" s="2"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" s="2">
         <v>19</v>
       </c>
@@ -2170,7 +2173,7 @@
       </c>
       <c r="C106" s="2"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" s="2">
         <v>20</v>
       </c>
@@ -2179,7 +2182,7 @@
       </c>
       <c r="C107" s="2"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" s="2">
         <v>21</v>
       </c>
@@ -2188,7 +2191,7 @@
       </c>
       <c r="C108" s="2"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" s="2">
         <v>22</v>
       </c>
@@ -2197,7 +2200,7 @@
       </c>
       <c r="C109" s="2"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" s="2">
         <v>23</v>
       </c>
@@ -2206,7 +2209,7 @@
       </c>
       <c r="C110" s="2"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" s="2">
         <v>24</v>
       </c>
@@ -2215,8 +2218,8 @@
       </c>
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="15" thickBot="1"/>
+    <row r="113" spans="1:3" ht="15" thickBot="1">
       <c r="A113" s="20" t="s">
         <v>2</v>
       </c>
@@ -2227,7 +2230,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="15" thickBot="1">
       <c r="A114" s="5">
         <v>5</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="15" thickBot="1">
       <c r="A115" s="20" t="s">
         <v>16</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" s="5">
         <v>1</v>
       </c>
@@ -2258,7 +2261,7 @@
       </c>
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" s="2">
         <v>2</v>
       </c>
@@ -2267,7 +2270,7 @@
       </c>
       <c r="C117" s="2"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" s="2">
         <v>3</v>
       </c>
@@ -2276,7 +2279,7 @@
       </c>
       <c r="C118" s="2"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" s="2">
         <v>4</v>
       </c>
@@ -2285,7 +2288,7 @@
       </c>
       <c r="C119" s="2"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" s="2">
         <v>5</v>
       </c>
@@ -2294,7 +2297,7 @@
       </c>
       <c r="C120" s="2"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" s="2">
         <v>6</v>
       </c>
@@ -2303,7 +2306,7 @@
       </c>
       <c r="C121" s="2"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" s="2">
         <v>7</v>
       </c>
@@ -2312,7 +2315,7 @@
       </c>
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" s="2">
         <v>8</v>
       </c>
@@ -2321,7 +2324,7 @@
       </c>
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" s="19">
         <v>9</v>
       </c>
@@ -2330,7 +2333,7 @@
       </c>
       <c r="C124" s="19"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" s="2">
         <v>10</v>
       </c>
@@ -2339,7 +2342,7 @@
       </c>
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" s="2">
         <v>11</v>
       </c>
@@ -2348,7 +2351,7 @@
       </c>
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" s="2">
         <v>12</v>
       </c>
@@ -2357,7 +2360,7 @@
       </c>
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" s="2">
         <v>13</v>
       </c>
@@ -2366,7 +2369,7 @@
       </c>
       <c r="C128" s="2"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3">
       <c r="A129" s="19">
         <v>14</v>
       </c>
@@ -2375,7 +2378,7 @@
       </c>
       <c r="C129" s="19"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3">
       <c r="A130" s="2">
         <v>15</v>
       </c>
@@ -2384,7 +2387,7 @@
       </c>
       <c r="C130" s="2"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3">
       <c r="A131" s="2">
         <v>16</v>
       </c>
@@ -2393,7 +2396,7 @@
       </c>
       <c r="C131" s="2"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3">
       <c r="A132" s="2">
         <v>17</v>
       </c>
@@ -2402,7 +2405,7 @@
       </c>
       <c r="C132" s="2"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3">
       <c r="A133" s="2">
         <v>18</v>
       </c>
@@ -2411,7 +2414,7 @@
       </c>
       <c r="C133" s="2"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3">
       <c r="A134" s="2">
         <v>19</v>
       </c>
@@ -2420,7 +2423,7 @@
       </c>
       <c r="C134" s="2"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3">
       <c r="A135" s="2">
         <v>20</v>
       </c>
@@ -2429,7 +2432,7 @@
       </c>
       <c r="C135" s="2"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3">
       <c r="A136" s="2">
         <v>21</v>
       </c>
@@ -2438,7 +2441,7 @@
       </c>
       <c r="C136" s="2"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3">
       <c r="A137" s="2">
         <v>22</v>
       </c>
@@ -2447,7 +2450,7 @@
       </c>
       <c r="C137" s="2"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3">
       <c r="A138" s="2">
         <v>23</v>
       </c>
@@ -2456,7 +2459,7 @@
       </c>
       <c r="C138" s="2"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3">
       <c r="A139" s="2">
         <v>24</v>
       </c>
@@ -2465,8 +2468,8 @@
       </c>
       <c r="C139" s="2"/>
     </row>
-    <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="15" thickBot="1"/>
+    <row r="141" spans="1:3" ht="15" thickBot="1">
       <c r="A141" s="20" t="s">
         <v>2</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="15" thickBot="1">
       <c r="A142" s="5">
         <v>6</v>
       </c>
@@ -2488,7 +2491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="15" thickBot="1">
       <c r="A143" s="20" t="s">
         <v>16</v>
       </c>
@@ -2499,7 +2502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3">
       <c r="A144" s="5">
         <v>1</v>
       </c>
@@ -2508,7 +2511,7 @@
       </c>
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3">
       <c r="A145" s="2">
         <v>2</v>
       </c>
@@ -2517,7 +2520,7 @@
       </c>
       <c r="C145" s="2"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3">
       <c r="A146" s="2">
         <v>3</v>
       </c>
@@ -2526,7 +2529,7 @@
       </c>
       <c r="C146" s="2"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3">
       <c r="A147" s="2">
         <v>4</v>
       </c>
@@ -2535,7 +2538,7 @@
       </c>
       <c r="C147" s="2"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3">
       <c r="A148" s="2">
         <v>5</v>
       </c>
@@ -2544,7 +2547,7 @@
       </c>
       <c r="C148" s="2"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3">
       <c r="A149" s="2">
         <v>6</v>
       </c>
@@ -2553,7 +2556,7 @@
       </c>
       <c r="C149" s="2"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3">
       <c r="A150" s="2">
         <v>7</v>
       </c>
@@ -2562,7 +2565,7 @@
       </c>
       <c r="C150" s="2"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3">
       <c r="A151" s="2">
         <v>8</v>
       </c>
@@ -2571,7 +2574,7 @@
       </c>
       <c r="C151" s="2"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3">
       <c r="A152" s="19">
         <v>9</v>
       </c>
@@ -2580,7 +2583,7 @@
       </c>
       <c r="C152" s="19"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3">
       <c r="A153" s="2">
         <v>10</v>
       </c>
@@ -2589,7 +2592,7 @@
       </c>
       <c r="C153" s="2"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3">
       <c r="A154" s="2">
         <v>11</v>
       </c>
@@ -2598,7 +2601,7 @@
       </c>
       <c r="C154" s="2"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3">
       <c r="A155" s="2">
         <v>12</v>
       </c>
@@ -2607,7 +2610,7 @@
       </c>
       <c r="C155" s="2"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3">
       <c r="A156" s="2">
         <v>13</v>
       </c>
@@ -2616,7 +2619,7 @@
       </c>
       <c r="C156" s="2"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3">
       <c r="A157" s="19">
         <v>14</v>
       </c>
@@ -2625,7 +2628,7 @@
       </c>
       <c r="C157" s="19"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3">
       <c r="A158" s="2">
         <v>15</v>
       </c>
@@ -2634,7 +2637,7 @@
       </c>
       <c r="C158" s="2"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3">
       <c r="A159" s="2">
         <v>16</v>
       </c>
@@ -2643,7 +2646,7 @@
       </c>
       <c r="C159" s="2"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3">
       <c r="A160" s="2">
         <v>17</v>
       </c>
@@ -2652,7 +2655,7 @@
       </c>
       <c r="C160" s="2"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3">
       <c r="A161" s="2">
         <v>18</v>
       </c>
@@ -2661,7 +2664,7 @@
       </c>
       <c r="C161" s="2"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3">
       <c r="A162" s="2">
         <v>19</v>
       </c>
@@ -2670,7 +2673,7 @@
       </c>
       <c r="C162" s="2"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3">
       <c r="A163" s="2">
         <v>20</v>
       </c>
@@ -2679,7 +2682,7 @@
       </c>
       <c r="C163" s="2"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3">
       <c r="A164" s="2">
         <v>21</v>
       </c>
@@ -2688,7 +2691,7 @@
       </c>
       <c r="C164" s="2"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3">
       <c r="A165" s="2">
         <v>22</v>
       </c>
@@ -2697,7 +2700,7 @@
       </c>
       <c r="C165" s="2"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3">
       <c r="A166" s="2">
         <v>23</v>
       </c>
@@ -2706,7 +2709,7 @@
       </c>
       <c r="C166" s="2"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3">
       <c r="A167" s="2">
         <v>24</v>
       </c>
@@ -2715,8 +2718,8 @@
       </c>
       <c r="C167" s="2"/>
     </row>
-    <row r="168" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="169" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="15" thickBot="1"/>
+    <row r="169" spans="1:3" ht="15" thickBot="1">
       <c r="A169" s="20" t="s">
         <v>2</v>
       </c>
@@ -2727,7 +2730,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="15" thickBot="1">
       <c r="A170" s="5">
         <v>7</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="15" thickBot="1">
       <c r="A171" s="20" t="s">
         <v>16</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3">
       <c r="A172" s="5">
         <v>1</v>
       </c>
@@ -2758,7 +2761,7 @@
       </c>
       <c r="C172" s="5"/>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3">
       <c r="A173" s="2">
         <v>2</v>
       </c>
@@ -2767,7 +2770,7 @@
       </c>
       <c r="C173" s="2"/>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3">
       <c r="A174" s="2">
         <v>3</v>
       </c>
@@ -2776,7 +2779,7 @@
       </c>
       <c r="C174" s="2"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3">
       <c r="A175" s="2">
         <v>4</v>
       </c>
@@ -2785,7 +2788,7 @@
       </c>
       <c r="C175" s="2"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3">
       <c r="A176" s="2">
         <v>5</v>
       </c>
@@ -2794,7 +2797,7 @@
       </c>
       <c r="C176" s="2"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3">
       <c r="A177" s="2">
         <v>6</v>
       </c>
@@ -2803,7 +2806,7 @@
       </c>
       <c r="C177" s="2"/>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3">
       <c r="A178" s="2">
         <v>7</v>
       </c>
@@ -2812,7 +2815,7 @@
       </c>
       <c r="C178" s="2"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3">
       <c r="A179" s="2">
         <v>8</v>
       </c>
@@ -2821,7 +2824,7 @@
       </c>
       <c r="C179" s="2"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3">
       <c r="A180" s="19">
         <v>9</v>
       </c>
@@ -2830,7 +2833,7 @@
       </c>
       <c r="C180" s="19"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3">
       <c r="A181" s="2">
         <v>10</v>
       </c>
@@ -2839,7 +2842,7 @@
       </c>
       <c r="C181" s="2"/>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3">
       <c r="A182" s="2">
         <v>11</v>
       </c>
@@ -2848,7 +2851,7 @@
       </c>
       <c r="C182" s="2"/>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3">
       <c r="A183" s="2">
         <v>12</v>
       </c>
@@ -2857,7 +2860,7 @@
       </c>
       <c r="C183" s="2"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3">
       <c r="A184" s="2">
         <v>13</v>
       </c>
@@ -2866,7 +2869,7 @@
       </c>
       <c r="C184" s="2"/>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3">
       <c r="A185" s="19">
         <v>14</v>
       </c>
@@ -2875,7 +2878,7 @@
       </c>
       <c r="C185" s="19"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3">
       <c r="A186" s="2">
         <v>15</v>
       </c>
@@ -2884,7 +2887,7 @@
       </c>
       <c r="C186" s="2"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3">
       <c r="A187" s="2">
         <v>16</v>
       </c>
@@ -2893,7 +2896,7 @@
       </c>
       <c r="C187" s="2"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3">
       <c r="A188" s="2">
         <v>17</v>
       </c>
@@ -2902,7 +2905,7 @@
       </c>
       <c r="C188" s="2"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3">
       <c r="A189" s="2">
         <v>18</v>
       </c>
@@ -2911,7 +2914,7 @@
       </c>
       <c r="C189" s="2"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3">
       <c r="A190" s="2">
         <v>19</v>
       </c>
@@ -2920,7 +2923,7 @@
       </c>
       <c r="C190" s="2"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3">
       <c r="A191" s="2">
         <v>20</v>
       </c>
@@ -2929,7 +2932,7 @@
       </c>
       <c r="C191" s="2"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3">
       <c r="A192" s="2">
         <v>21</v>
       </c>
@@ -2938,7 +2941,7 @@
       </c>
       <c r="C192" s="2"/>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3">
       <c r="A193" s="2">
         <v>22</v>
       </c>
@@ -2947,7 +2950,7 @@
       </c>
       <c r="C193" s="2"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3">
       <c r="A194" s="2">
         <v>23</v>
       </c>
@@ -2956,7 +2959,7 @@
       </c>
       <c r="C194" s="2"/>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3">
       <c r="A195" s="2">
         <v>24</v>
       </c>
@@ -2965,8 +2968,8 @@
       </c>
       <c r="C195" s="2"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="197" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="15" thickBot="1"/>
+    <row r="197" spans="1:3" ht="15" thickBot="1">
       <c r="A197" s="20" t="s">
         <v>2</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="15" thickBot="1">
       <c r="A198" s="5">
         <v>8</v>
       </c>
@@ -2988,7 +2991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="15" thickBot="1">
       <c r="A199" s="20" t="s">
         <v>16</v>
       </c>
@@ -2999,7 +3002,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3">
       <c r="A200" s="5">
         <v>1</v>
       </c>
@@ -3008,7 +3011,7 @@
       </c>
       <c r="C200" s="5"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3">
       <c r="A201" s="2">
         <v>2</v>
       </c>
@@ -3017,7 +3020,7 @@
       </c>
       <c r="C201" s="2"/>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3">
       <c r="A202" s="2">
         <v>3</v>
       </c>
@@ -3026,7 +3029,7 @@
       </c>
       <c r="C202" s="2"/>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3">
       <c r="A203" s="2">
         <v>4</v>
       </c>
@@ -3035,7 +3038,7 @@
       </c>
       <c r="C203" s="2"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3">
       <c r="A204" s="2">
         <v>5</v>
       </c>
@@ -3044,7 +3047,7 @@
       </c>
       <c r="C204" s="2"/>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3">
       <c r="A205" s="2">
         <v>6</v>
       </c>
@@ -3053,7 +3056,7 @@
       </c>
       <c r="C205" s="2"/>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3">
       <c r="A206" s="2">
         <v>7</v>
       </c>
@@ -3062,7 +3065,7 @@
       </c>
       <c r="C206" s="2"/>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3">
       <c r="A207" s="2">
         <v>8</v>
       </c>
@@ -3071,7 +3074,7 @@
       </c>
       <c r="C207" s="2"/>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3">
       <c r="A208" s="19">
         <v>9</v>
       </c>
@@ -3080,7 +3083,7 @@
       </c>
       <c r="C208" s="19"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3">
       <c r="A209" s="2">
         <v>10</v>
       </c>
@@ -3089,7 +3092,7 @@
       </c>
       <c r="C209" s="2"/>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3">
       <c r="A210" s="2">
         <v>11</v>
       </c>
@@ -3098,7 +3101,7 @@
       </c>
       <c r="C210" s="2"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3">
       <c r="A211" s="2">
         <v>12</v>
       </c>
@@ -3107,7 +3110,7 @@
       </c>
       <c r="C211" s="2"/>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3">
       <c r="A212" s="2">
         <v>13</v>
       </c>
@@ -3116,7 +3119,7 @@
       </c>
       <c r="C212" s="2"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3">
       <c r="A213" s="19">
         <v>14</v>
       </c>
@@ -3125,7 +3128,7 @@
       </c>
       <c r="C213" s="19"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3">
       <c r="A214" s="2">
         <v>15</v>
       </c>
@@ -3134,7 +3137,7 @@
       </c>
       <c r="C214" s="2"/>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3">
       <c r="A215" s="2">
         <v>16</v>
       </c>
@@ -3143,7 +3146,7 @@
       </c>
       <c r="C215" s="2"/>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3">
       <c r="A216" s="2">
         <v>17</v>
       </c>
@@ -3152,7 +3155,7 @@
       </c>
       <c r="C216" s="2"/>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3">
       <c r="A217" s="2">
         <v>18</v>
       </c>
@@ -3161,7 +3164,7 @@
       </c>
       <c r="C217" s="2"/>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3">
       <c r="A218" s="2">
         <v>19</v>
       </c>
@@ -3170,7 +3173,7 @@
       </c>
       <c r="C218" s="2"/>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3">
       <c r="A219" s="2">
         <v>20</v>
       </c>
@@ -3179,7 +3182,7 @@
       </c>
       <c r="C219" s="2"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3">
       <c r="A220" s="2">
         <v>21</v>
       </c>
@@ -3188,7 +3191,7 @@
       </c>
       <c r="C220" s="2"/>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3">
       <c r="A221" s="2">
         <v>22</v>
       </c>
@@ -3197,7 +3200,7 @@
       </c>
       <c r="C221" s="2"/>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3">
       <c r="A222" s="2">
         <v>23</v>
       </c>
@@ -3206,7 +3209,7 @@
       </c>
       <c r="C222" s="2"/>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3">
       <c r="A223" s="2">
         <v>24</v>
       </c>

</xml_diff>